<commit_message>
add function creating new lesson and hits for choose date freeze bot for 1 request in second
</commit_message>
<xml_diff>
--- a/attendance.xlsx
+++ b/attendance.xlsx
@@ -7,7 +7,6 @@
   </bookViews>
   <sheets>
     <sheet name="2022-2023" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="1 rehc" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -16,8 +15,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -77,7 +77,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
@@ -86,6 +86,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -430,10 +432,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T151"/>
+  <dimension ref="A1:V149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="76" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="76" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -470,50 +472,60 @@
           <t>Достижения</t>
         </is>
       </c>
-      <c r="E1" s="4" t="n">
+      <c r="E1" s="5" t="n">
         <v>44828</v>
       </c>
-      <c r="F1" s="4" t="n">
+      <c r="F1" s="5" t="n">
         <v>44835</v>
       </c>
-      <c r="G1" s="4" t="n">
+      <c r="G1" s="5" t="n">
         <v>44842</v>
       </c>
-      <c r="H1" s="4" t="n">
+      <c r="H1" s="5" t="n">
         <v>44849</v>
       </c>
-      <c r="I1" s="4" t="n">
+      <c r="I1" s="5" t="n">
         <v>44856</v>
       </c>
-      <c r="J1" s="4" t="n">
+      <c r="J1" s="5" t="n">
         <v>44863</v>
       </c>
-      <c r="K1" s="4" t="n">
+      <c r="K1" s="5" t="n">
         <v>44870</v>
       </c>
-      <c r="L1" s="4" t="n">
+      <c r="L1" s="5" t="n">
         <v>44846</v>
       </c>
-      <c r="M1" s="4" t="n">
+      <c r="M1" s="5" t="n">
         <v>44853</v>
       </c>
-      <c r="N1" s="4" t="n">
+      <c r="N1" s="5" t="n">
         <v>44891</v>
       </c>
-      <c r="O1" s="4" t="n">
+      <c r="O1" s="5" t="n">
         <v>44898</v>
       </c>
-      <c r="P1" s="4" t="n">
+      <c r="P1" s="5" t="n">
         <v>44905</v>
       </c>
-      <c r="Q1" s="4" t="n">
+      <c r="Q1" s="5" t="n">
         <v>44912</v>
       </c>
-      <c r="R1" s="4" t="n">
+      <c r="R1" s="5" t="n">
         <v>44919</v>
       </c>
-      <c r="S1" s="4" t="n"/>
-      <c r="T1" s="4" t="n"/>
+      <c r="S1" s="5" t="n">
+        <v>38028</v>
+      </c>
+      <c r="T1" s="5" t="n">
+        <v>44856</v>
+      </c>
+      <c r="U1" s="6" t="n">
+        <v>44906</v>
+      </c>
+      <c r="V1" s="5" t="n">
+        <v>44905</v>
+      </c>
     </row>
     <row r="2" ht="15" customHeight="1" thickBot="1">
       <c r="B2" t="n">
@@ -524,6 +536,11 @@
           <t>Акрами</t>
         </is>
       </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>+</t>
+        </is>
+      </c>
     </row>
     <row r="3" ht="15" customHeight="1" thickBot="1">
       <c r="B3" t="n">
@@ -534,6 +551,8 @@
           <t>Амельченко</t>
         </is>
       </c>
+      <c r="S3" s="5" t="n"/>
+      <c r="T3" s="5" t="n"/>
     </row>
     <row r="4" ht="15" customHeight="1" thickBot="1">
       <c r="B4" t="n">
@@ -574,6 +593,21 @@
           <t>Афанасьев</t>
         </is>
       </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>+</t>
+        </is>
+      </c>
+      <c r="S7" t="inlineStr">
+        <is>
+          <t>+</t>
+        </is>
+      </c>
+      <c r="U7" t="inlineStr">
+        <is>
+          <t>+</t>
+        </is>
+      </c>
     </row>
     <row r="8" ht="15" customHeight="1" thickBot="1">
       <c r="B8" t="n">
@@ -587,6 +621,11 @@
       <c r="D8" t="inlineStr">
         <is>
           <t xml:space="preserve"> 2 разряд</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>+</t>
         </is>
       </c>
     </row>
@@ -772,9 +811,6 @@
       </c>
     </row>
     <row r="26" ht="15" customHeight="1" thickBot="1">
-      <c r="A26" t="n">
-        <v>5407115545</v>
-      </c>
       <c r="B26" t="n">
         <v>1</v>
       </c>
@@ -1006,11 +1042,6 @@
           <t>Жуков</t>
         </is>
       </c>
-      <c r="T46" t="inlineStr">
-        <is>
-          <t>+</t>
-        </is>
-      </c>
     </row>
     <row r="47" ht="15" customHeight="1" thickBot="1">
       <c r="B47" t="n">
@@ -2114,41 +2145,6 @@
       <c r="C149" s="2" t="inlineStr">
         <is>
           <t>Шутов</t>
-        </is>
-      </c>
-    </row>
-    <row r="150">
-      <c r="B150" t="n">
-        <v>1</v>
-      </c>
-      <c r="C150" t="inlineStr">
-        <is>
-          <t>:::::</t>
-        </is>
-      </c>
-      <c r="E150" t="inlineStr">
-        <is>
-          <t>+</t>
-        </is>
-      </c>
-      <c r="P150" t="inlineStr">
-        <is>
-          <t>+</t>
-        </is>
-      </c>
-    </row>
-    <row r="151">
-      <c r="B151" t="n">
-        <v>2</v>
-      </c>
-      <c r="C151" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="D151" t="inlineStr">
-        <is>
-          <t>23</t>
         </is>
       </c>
     </row>
@@ -2156,928 +2152,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9" horizontalDpi="4294967293" verticalDpi="0"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:T75"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>chat id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Курс</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Шахматист</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Достижения</t>
-        </is>
-      </c>
-      <c r="E1" s="4" t="n">
-        <v>44856</v>
-      </c>
-      <c r="F1" s="4" t="n">
-        <v>44863</v>
-      </c>
-      <c r="G1" s="4" t="n">
-        <v>44870</v>
-      </c>
-      <c r="H1" s="4" t="n">
-        <v>44877</v>
-      </c>
-      <c r="I1" s="4" t="n">
-        <v>44884</v>
-      </c>
-      <c r="J1" s="4" t="n">
-        <v>44891</v>
-      </c>
-      <c r="K1" s="4" t="n">
-        <v>44898</v>
-      </c>
-      <c r="L1" s="4" t="n">
-        <v>44905</v>
-      </c>
-      <c r="M1" s="4" t="n">
-        <v>44912</v>
-      </c>
-      <c r="N1" s="4" t="n">
-        <v>44919</v>
-      </c>
-      <c r="O1" s="4" t="n">
-        <v>44926</v>
-      </c>
-      <c r="P1" s="4" t="n">
-        <v>44933</v>
-      </c>
-      <c r="Q1" s="4" t="n">
-        <v>44940</v>
-      </c>
-      <c r="R1" s="4" t="n">
-        <v>44947</v>
-      </c>
-      <c r="S1" s="4" t="n">
-        <v>44954</v>
-      </c>
-      <c r="T1" s="4" t="n">
-        <v>44961</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="B2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Афанасьев</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="B3" t="n">
-        <v>1</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Афти</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 2 разряд</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="B4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Бадокина</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="B5" t="n">
-        <v>1</v>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Барсегян</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="B6" t="n">
-        <v>1</v>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Безденежных</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="B7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Берко</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="B8" t="n">
-        <v>1</v>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Богатов</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 2 разряд</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="B9" t="n">
-        <v>1</v>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Богданова</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="B10" t="n">
-        <v>1</v>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Бородин Максим Юрьевич</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="B11" t="n">
-        <v>1</v>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Васильев</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="B12" t="n">
-        <v>1</v>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Величко</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 2 разряд</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="B13" t="n">
-        <v>1</v>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Гайворонский</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="B14" t="n">
-        <v>1</v>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>Глаголев</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 1 разряд</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="B15" t="n">
-        <v>1</v>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>Глинская</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="B16" t="n">
-        <v>1</v>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Голионцев </t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>2 разряд</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="B17" t="n">
-        <v>1</v>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>Голицын</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 2 разряд</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="B18" t="n">
-        <v>1</v>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>Григорьева</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="B19" t="n">
-        <v>1</v>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>Гурьянов</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="B20" t="n">
-        <v>1</v>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Гусев </t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>3 разряд</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="B21" t="n">
-        <v>1</v>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>Дорожкина</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="B22" t="n">
-        <v>1</v>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>Драчкова</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="B23" t="n">
-        <v>1</v>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>Жуков</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>+</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="B24" t="n">
-        <v>1</v>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>Зайцева</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="B25" t="n">
-        <v>1</v>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Зарипов </t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>2 разряд</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="B26" t="n">
-        <v>1</v>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>Зернов</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="B27" t="n">
-        <v>1</v>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>Зияудинов</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="B28" t="n">
-        <v>1</v>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>Капский</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="B29" t="n">
-        <v>1</v>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>Кастусик</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="B30" t="n">
-        <v>1</v>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>Качина</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="B31" t="n">
-        <v>1</v>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>Киселев</t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 2 разряд</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="B32" t="n">
-        <v>1</v>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>Кияткин</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="B33" t="n">
-        <v>1</v>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>Коваленко</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="B34" t="n">
-        <v>1</v>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>Ковальчук</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="B35" t="n">
-        <v>1</v>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Колядинцев </t>
-        </is>
-      </c>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>1 разряд</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="B36" t="n">
-        <v>1</v>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>Кондратьева</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="B37" t="n">
-        <v>1</v>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>Кормановский</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="B38" t="n">
-        <v>1</v>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>Коханович</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="B39" t="n">
-        <v>1</v>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>Красовский</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="B40" t="n">
-        <v>1</v>
-      </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>Кузьмин</t>
-        </is>
-      </c>
-    </row>
-    <row r="41">
-      <c r="B41" t="n">
-        <v>1</v>
-      </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t>Кулешов</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="B42" t="n">
-        <v>1</v>
-      </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Куликов </t>
-        </is>
-      </c>
-      <c r="D42" t="inlineStr">
-        <is>
-          <t>1 разряд</t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
-      <c r="B43" t="n">
-        <v>1</v>
-      </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>Кулов</t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
-      <c r="B44" t="n">
-        <v>1</v>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>Кургузов</t>
-        </is>
-      </c>
-    </row>
-    <row r="45">
-      <c r="B45" t="n">
-        <v>1</v>
-      </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>Лушин</t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="B46" t="n">
-        <v>1</v>
-      </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>Макаров</t>
-        </is>
-      </c>
-    </row>
-    <row r="47">
-      <c r="B47" t="n">
-        <v>1</v>
-      </c>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t>Марченко</t>
-        </is>
-      </c>
-    </row>
-    <row r="48">
-      <c r="B48" t="n">
-        <v>1</v>
-      </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>Меленьтев</t>
-        </is>
-      </c>
-      <c r="D48" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 1 разряд</t>
-        </is>
-      </c>
-    </row>
-    <row r="49">
-      <c r="B49" t="n">
-        <v>1</v>
-      </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t>Михнин</t>
-        </is>
-      </c>
-    </row>
-    <row r="50">
-      <c r="B50" t="n">
-        <v>1</v>
-      </c>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t>Молдавский</t>
-        </is>
-      </c>
-    </row>
-    <row r="51">
-      <c r="B51" t="n">
-        <v>1</v>
-      </c>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t>Молотов</t>
-        </is>
-      </c>
-    </row>
-    <row r="52">
-      <c r="B52" t="n">
-        <v>1</v>
-      </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Музафаров </t>
-        </is>
-      </c>
-      <c r="D52" t="inlineStr">
-        <is>
-          <t>1 разряд</t>
-        </is>
-      </c>
-    </row>
-    <row r="53">
-      <c r="B53" t="n">
-        <v>1</v>
-      </c>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Органдейкина </t>
-        </is>
-      </c>
-      <c r="D53" t="inlineStr">
-        <is>
-          <t>2 разряд</t>
-        </is>
-      </c>
-    </row>
-    <row r="54">
-      <c r="B54" t="n">
-        <v>1</v>
-      </c>
-      <c r="C54" t="inlineStr">
-        <is>
-          <t>Осокин</t>
-        </is>
-      </c>
-    </row>
-    <row r="55">
-      <c r="B55" t="n">
-        <v>1</v>
-      </c>
-      <c r="C55" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Паюсов </t>
-        </is>
-      </c>
-      <c r="D55" t="inlineStr">
-        <is>
-          <t>2 разряд</t>
-        </is>
-      </c>
-    </row>
-    <row r="56">
-      <c r="B56" t="n">
-        <v>1</v>
-      </c>
-      <c r="C56" t="inlineStr">
-        <is>
-          <t>Плеханова</t>
-        </is>
-      </c>
-    </row>
-    <row r="57">
-      <c r="B57" t="n">
-        <v>1</v>
-      </c>
-      <c r="C57" t="inlineStr">
-        <is>
-          <t>Подольская</t>
-        </is>
-      </c>
-    </row>
-    <row r="58">
-      <c r="B58" t="n">
-        <v>1</v>
-      </c>
-      <c r="C58" t="inlineStr">
-        <is>
-          <t>Подрешетников</t>
-        </is>
-      </c>
-      <c r="D58" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 1 разряд</t>
-        </is>
-      </c>
-    </row>
-    <row r="59">
-      <c r="B59" t="n">
-        <v>1</v>
-      </c>
-      <c r="C59" t="inlineStr">
-        <is>
-          <t>Порецков</t>
-        </is>
-      </c>
-    </row>
-    <row r="60">
-      <c r="B60" t="n">
-        <v>1</v>
-      </c>
-      <c r="C60" t="inlineStr">
-        <is>
-          <t>Пумпур</t>
-        </is>
-      </c>
-    </row>
-    <row r="61">
-      <c r="B61" t="n">
-        <v>1</v>
-      </c>
-      <c r="C61" t="inlineStr">
-        <is>
-          <t>Пьянков</t>
-        </is>
-      </c>
-    </row>
-    <row r="62">
-      <c r="B62" t="n">
-        <v>1</v>
-      </c>
-      <c r="C62" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Салимшин </t>
-        </is>
-      </c>
-      <c r="D62" t="inlineStr">
-        <is>
-          <t>1 разряд</t>
-        </is>
-      </c>
-    </row>
-    <row r="63">
-      <c r="B63" t="n">
-        <v>1</v>
-      </c>
-      <c r="C63" t="inlineStr">
-        <is>
-          <t>Саунин</t>
-        </is>
-      </c>
-    </row>
-    <row r="64">
-      <c r="B64" t="n">
-        <v>1</v>
-      </c>
-      <c r="C64" t="inlineStr">
-        <is>
-          <t>Сафонова</t>
-        </is>
-      </c>
-    </row>
-    <row r="65">
-      <c r="B65" t="n">
-        <v>1</v>
-      </c>
-      <c r="C65" t="inlineStr">
-        <is>
-          <t>Сивкова</t>
-        </is>
-      </c>
-    </row>
-    <row r="66">
-      <c r="B66" t="n">
-        <v>1</v>
-      </c>
-      <c r="C66" t="inlineStr">
-        <is>
-          <t>Смолин</t>
-        </is>
-      </c>
-    </row>
-    <row r="67">
-      <c r="B67" t="n">
-        <v>1</v>
-      </c>
-      <c r="C67" t="inlineStr">
-        <is>
-          <t>Сташевская</t>
-        </is>
-      </c>
-    </row>
-    <row r="68">
-      <c r="B68" t="n">
-        <v>1</v>
-      </c>
-      <c r="C68" t="inlineStr">
-        <is>
-          <t>Тимофеев</t>
-        </is>
-      </c>
-    </row>
-    <row r="69">
-      <c r="B69" t="n">
-        <v>1</v>
-      </c>
-      <c r="C69" t="inlineStr">
-        <is>
-          <t>Фахриев</t>
-        </is>
-      </c>
-    </row>
-    <row r="70">
-      <c r="B70" t="n">
-        <v>1</v>
-      </c>
-      <c r="C70" t="inlineStr">
-        <is>
-          <t>Федорова</t>
-        </is>
-      </c>
-    </row>
-    <row r="71">
-      <c r="B71" t="n">
-        <v>1</v>
-      </c>
-      <c r="C71" t="inlineStr">
-        <is>
-          <t>Цыбульник</t>
-        </is>
-      </c>
-    </row>
-    <row r="72">
-      <c r="B72" t="n">
-        <v>1</v>
-      </c>
-      <c r="C72" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Чекан </t>
-        </is>
-      </c>
-      <c r="D72" t="inlineStr">
-        <is>
-          <t>2 разряд</t>
-        </is>
-      </c>
-    </row>
-    <row r="73">
-      <c r="B73" t="n">
-        <v>1</v>
-      </c>
-      <c r="C73" t="inlineStr">
-        <is>
-          <t>Чирковский</t>
-        </is>
-      </c>
-    </row>
-    <row r="74">
-      <c r="B74" t="n">
-        <v>1</v>
-      </c>
-      <c r="C74" t="inlineStr">
-        <is>
-          <t>Шавруков</t>
-        </is>
-      </c>
-    </row>
-    <row r="75">
-      <c r="B75" t="n">
-        <v>1</v>
-      </c>
-      <c r="C75" t="inlineStr">
-        <is>
-          <t>Шуберт</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>